<commit_message>
Umeå -- allow patientID format 19120506-1234 (remove '-' characters before hashing)
</commit_message>
<xml_diff>
--- a/EUCANIMAGE_UMU_Subject_Tracker.xlsx
+++ b/EUCANIMAGE_UMU_Subject_Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\EUCanImage_skript_repo\Hashing-512-256\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8884692C-3F6B-45C1-B2BF-A44EA06A2561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDCCC9D9-86BA-4C2A-A0CA-8122DD03AC61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5665" yWindow="3722" windowWidth="26857" windowHeight="13449" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10528" yWindow="5271" windowWidth="20187" windowHeight="11330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tracker" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="428">
   <si>
     <t>EUCAN ID</t>
   </si>
@@ -1302,6 +1302,9 @@
   </si>
   <si>
     <t>ECI_UMU_S0404</t>
+  </si>
+  <si>
+    <t>1912-12121220</t>
   </si>
 </sst>
 </file>
@@ -1851,7 +1854,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15.8" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2038,6 +2041,9 @@
       <c r="I10" s="9"/>
     </row>
     <row r="11" spans="1:9" ht="15.8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>427</v>
+      </c>
       <c r="B11" t="s">
         <v>36</v>
       </c>

</xml_diff>